<commit_message>
last commit before graduation
seems like legit 1.0 release
</commit_message>
<xml_diff>
--- a/locales/LogicGates.xlsx
+++ b/locales/LogicGates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Godot Projects\games\LogicGates\locales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66FFA3E-9356-4296-A659-994FE24AD9AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7759B1B3-BABF-42DB-81F8-73EB902A9D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{93BF285B-5C8A-4A49-BC21-EB10DDB396B6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="100">
   <si>
     <t>id</t>
   </si>
@@ -295,6 +295,36 @@
   </si>
   <si>
     <t>Открыть файл</t>
+  </si>
+  <si>
+    <t>Zoom Out</t>
+  </si>
+  <si>
+    <t>Zoom Reset</t>
+  </si>
+  <si>
+    <t>Zoom In</t>
+  </si>
+  <si>
+    <t>Enable snap and show grid.</t>
+  </si>
+  <si>
+    <t>Enable grid minimap.</t>
+  </si>
+  <si>
+    <t>Уменьшить масштаб</t>
+  </si>
+  <si>
+    <t>Сбросить масштаб</t>
+  </si>
+  <si>
+    <t>Увеличить масштаб</t>
+  </si>
+  <si>
+    <t>Переключить видимость миникарты</t>
+  </si>
+  <si>
+    <t>Переключить прилипание и видимость сетки</t>
   </si>
 </sst>
 </file>
@@ -658,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C01293A-6D9E-470D-AE58-CB73C9E08F7F}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,6 +1096,61 @@
         <v>89</v>
       </c>
     </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>